<commit_message>
Revisão e preparação de Entrega 1 (rever por restantes membros)
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TrabalhosPraticos\Projeto Aplicado\ipca_gym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BFDF22-E251-44D3-8048-602ECF65727E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BACFDBF-DEF9-4044-A424-CDC4C957DCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -774,13 +774,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,18 +784,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -823,6 +805,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1122,8 +1122,8 @@
   </sheetPr>
   <dimension ref="A2:AP112"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" sqref="E34:F35"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1162,43 +1162,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="55"/>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="55"/>
-      <c r="AD2" s="55"/>
-      <c r="AE2" s="55"/>
-      <c r="AF2" s="55"/>
-      <c r="AG2" s="55"/>
-      <c r="AH2" s="55"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="49"/>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="49"/>
+      <c r="AH2" s="49"/>
     </row>
     <row r="5" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="50" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2">
@@ -1258,7 +1258,7 @@
       <c r="AH5"/>
     </row>
     <row r="6" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C6" s="56"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1315,8 +1315,8 @@
       <c r="AG6"/>
       <c r="AH6"/>
     </row>
-    <row r="7" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C7" s="56"/>
+    <row r="7" spans="2:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="50"/>
       <c r="D7" s="42" t="s">
         <v>53</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="K7" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="53"/>
+      <c r="L7" s="44"/>
       <c r="M7" s="43"/>
       <c r="N7" s="21" t="s">
         <v>57</v>
@@ -1396,7 +1396,7 @@
       <c r="AH8" s="12"/>
     </row>
     <row r="9" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="19">
@@ -1440,7 +1440,7 @@
       </c>
     </row>
     <row r="10" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C10" s="57"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="19" t="s">
         <v>5</v>
       </c>
@@ -1482,7 +1482,7 @@
       </c>
     </row>
     <row r="11" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="57"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="42" t="s">
         <v>24</v>
       </c>
@@ -1512,7 +1512,7 @@
       <c r="P11" s="15"/>
     </row>
     <row r="12" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C12" s="57"/>
+      <c r="C12" s="51"/>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
@@ -1529,7 +1529,7 @@
       <c r="AI12" s="7"/>
     </row>
     <row r="13" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C13" s="57"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="19">
         <v>14</v>
       </c>
@@ -1571,7 +1571,7 @@
       </c>
     </row>
     <row r="14" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C14" s="57"/>
+      <c r="C14" s="51"/>
       <c r="D14" s="27" t="s">
         <v>4</v>
       </c>
@@ -1618,13 +1618,13 @@
       <c r="AP14" s="1"/>
     </row>
     <row r="15" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="57"/>
+      <c r="C15" s="51"/>
       <c r="D15" s="20"/>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="47"/>
       <c r="H15" s="17"/>
       <c r="I15" s="42" t="s">
         <v>71</v>
@@ -1656,11 +1656,11 @@
     </row>
     <row r="16" spans="2:42" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="57"/>
+      <c r="C16" s="51"/>
     </row>
     <row r="17" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="57"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="19">
         <v>27</v>
       </c>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="18" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="57"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="19" t="s">
         <v>3</v>
       </c>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="19" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="57"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="42" t="s">
         <v>79</v>
       </c>
@@ -1713,7 +1713,7 @@
       <c r="B20" s="1"/>
     </row>
     <row r="21" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="57" t="s">
+      <c r="C21" s="51" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="19">
@@ -1758,7 +1758,7 @@
       <c r="AH21" s="12"/>
     </row>
     <row r="22" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="57"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="19" t="s">
         <v>6</v>
       </c>
@@ -1801,7 +1801,7 @@
       <c r="AH22" s="12"/>
     </row>
     <row r="23" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="57"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="21" t="s">
         <v>74</v>
       </c>
@@ -1826,7 +1826,7 @@
       <c r="AH23" s="12"/>
     </row>
     <row r="24" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="57"/>
+      <c r="C24" s="51"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
@@ -1860,7 +1860,7 @@
       <c r="AH24" s="14"/>
     </row>
     <row r="25" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="57"/>
+      <c r="C25" s="51"/>
       <c r="D25" s="19">
         <v>14</v>
       </c>
@@ -1914,7 +1914,7 @@
       </c>
     </row>
     <row r="26" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="57"/>
+      <c r="C26" s="51"/>
       <c r="D26" s="19" t="s">
         <v>1</v>
       </c>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="27" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27"/>
-      <c r="C27" s="57"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="42" t="s">
         <v>94</v>
       </c>
@@ -1987,12 +1987,12 @@
       <c r="L27" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="M27" s="53"/>
-      <c r="N27" s="53"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
       <c r="O27" s="43"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="59"/>
-      <c r="R27" s="60"/>
+      <c r="P27" s="52"/>
+      <c r="Q27" s="53"/>
+      <c r="R27" s="54"/>
       <c r="S27" s="42" t="s">
         <v>85</v>
       </c>
@@ -2205,45 +2205,45 @@
       </c>
       <c r="E31" s="43"/>
       <c r="F31" s="15"/>
-      <c r="G31" s="47" t="s">
+      <c r="G31" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="49"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="47"/>
       <c r="K31" s="16"/>
       <c r="L31" s="38" t="s">
         <v>18</v>
       </c>
       <c r="M31" s="16"/>
-      <c r="N31" s="47" t="s">
+      <c r="N31" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="O31" s="48"/>
-      <c r="P31" s="48"/>
-      <c r="Q31" s="48"/>
-      <c r="R31" s="49"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46"/>
+      <c r="R31" s="47"/>
       <c r="S31" s="40"/>
       <c r="T31" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="U31" s="53"/>
-      <c r="V31" s="53"/>
+      <c r="U31" s="44"/>
+      <c r="V31" s="44"/>
       <c r="W31" s="43"/>
-      <c r="X31" s="50"/>
-      <c r="Y31" s="51"/>
-      <c r="Z31" s="52"/>
+      <c r="X31" s="58"/>
+      <c r="Y31" s="59"/>
+      <c r="Z31" s="60"/>
       <c r="AA31" s="16"/>
-      <c r="AB31" s="44" t="s">
+      <c r="AB31" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="AC31" s="46"/>
+      <c r="AC31" s="57"/>
       <c r="AD31" s="18"/>
-      <c r="AE31" s="44" t="s">
+      <c r="AE31" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="AF31" s="45"/>
-      <c r="AG31" s="46"/>
+      <c r="AF31" s="56"/>
+      <c r="AG31" s="57"/>
       <c r="AH31" s="16"/>
     </row>
     <row r="32" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2425,12 +2425,12 @@
         <v>19</v>
       </c>
       <c r="J35" s="16"/>
-      <c r="K35" s="44" t="s">
+      <c r="K35" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="L35" s="45"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="46"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="57"/>
       <c r="O35" s="15"/>
       <c r="P35" s="38" t="s">
         <v>20</v>
@@ -3623,12 +3623,13 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="AB31:AC31"/>
+    <mergeCell ref="AE31:AG31"/>
+    <mergeCell ref="N31:R31"/>
+    <mergeCell ref="X31:Z31"/>
+    <mergeCell ref="T31:W31"/>
     <mergeCell ref="S27:T27"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="G31:J31"/>
@@ -3645,13 +3646,12 @@
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="P27:R27"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="AB31:AC31"/>
-    <mergeCell ref="AE31:AG31"/>
-    <mergeCell ref="N31:R31"/>
-    <mergeCell ref="X31:Z31"/>
-    <mergeCell ref="T31:W31"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Diagrama de Componentes + Organização Repositório
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TrabalhosPraticos\Projeto Aplicado\ipca_gym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DB3B19-93CC-4367-B00F-47997ECD086B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF04F67D-AB22-4D40-B822-806B60EF2CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma_Projecto" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="101">
   <si>
     <t>Dom</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>To-Do</t>
+  </si>
+  <si>
+    <t>Doing</t>
   </si>
 </sst>
 </file>
@@ -777,7 +780,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -787,6 +796,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -808,24 +829,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1165,43 +1168,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
-      <c r="AE2" s="49"/>
-      <c r="AF2" s="49"/>
-      <c r="AG2" s="49"/>
-      <c r="AH2" s="49"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="55"/>
+      <c r="AC2" s="55"/>
+      <c r="AD2" s="55"/>
+      <c r="AE2" s="55"/>
+      <c r="AF2" s="55"/>
+      <c r="AG2" s="55"/>
+      <c r="AH2" s="55"/>
     </row>
     <row r="5" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="56" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2">
@@ -1261,7 +1264,7 @@
       <c r="AH5"/>
     </row>
     <row r="6" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C6" s="50"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1319,7 +1322,7 @@
       <c r="AH6"/>
     </row>
     <row r="7" spans="2:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="50"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="42" t="s">
         <v>53</v>
       </c>
@@ -1338,7 +1341,7 @@
       <c r="K7" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="44"/>
+      <c r="L7" s="53"/>
       <c r="M7" s="43"/>
       <c r="N7" s="21" t="s">
         <v>57</v>
@@ -1399,7 +1402,7 @@
       <c r="AH8" s="12"/>
     </row>
     <row r="9" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="57" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="19">
@@ -1443,7 +1446,7 @@
       </c>
     </row>
     <row r="10" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C10" s="51"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="19" t="s">
         <v>5</v>
       </c>
@@ -1485,7 +1488,7 @@
       </c>
     </row>
     <row r="11" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="51"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="42" t="s">
         <v>24</v>
       </c>
@@ -1515,7 +1518,7 @@
       <c r="P11" s="15"/>
     </row>
     <row r="12" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C12" s="51"/>
+      <c r="C12" s="57"/>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
@@ -1532,7 +1535,7 @@
       <c r="AI12" s="7"/>
     </row>
     <row r="13" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C13" s="51"/>
+      <c r="C13" s="57"/>
       <c r="D13" s="19">
         <v>14</v>
       </c>
@@ -1574,7 +1577,7 @@
       </c>
     </row>
     <row r="14" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C14" s="51"/>
+      <c r="C14" s="57"/>
       <c r="D14" s="27" t="s">
         <v>4</v>
       </c>
@@ -1621,13 +1624,13 @@
       <c r="AP14" s="1"/>
     </row>
     <row r="15" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="51"/>
+      <c r="C15" s="57"/>
       <c r="D15" s="20"/>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="47"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="49"/>
       <c r="H15" s="17"/>
       <c r="I15" s="42" t="s">
         <v>71</v>
@@ -1659,11 +1662,11 @@
     </row>
     <row r="16" spans="2:42" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="51"/>
+      <c r="C16" s="57"/>
     </row>
     <row r="17" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="51"/>
+      <c r="C17" s="57"/>
       <c r="D17" s="19">
         <v>27</v>
       </c>
@@ -1682,7 +1685,7 @@
     </row>
     <row r="18" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="51"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="19" t="s">
         <v>3</v>
       </c>
@@ -1701,7 +1704,7 @@
     </row>
     <row r="19" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="51"/>
+      <c r="C19" s="57"/>
       <c r="D19" s="42" t="s">
         <v>79</v>
       </c>
@@ -1716,7 +1719,7 @@
       <c r="B20" s="1"/>
     </row>
     <row r="21" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="51" t="s">
+      <c r="C21" s="57" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="19">
@@ -1761,7 +1764,7 @@
       <c r="AH21" s="12"/>
     </row>
     <row r="22" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="51"/>
+      <c r="C22" s="57"/>
       <c r="D22" s="19" t="s">
         <v>6</v>
       </c>
@@ -1804,7 +1807,7 @@
       <c r="AH22" s="12"/>
     </row>
     <row r="23" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="51"/>
+      <c r="C23" s="57"/>
       <c r="D23" s="21" t="s">
         <v>74</v>
       </c>
@@ -1829,7 +1832,7 @@
       <c r="AH23" s="12"/>
     </row>
     <row r="24" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="51"/>
+      <c r="C24" s="57"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
@@ -1863,7 +1866,7 @@
       <c r="AH24" s="14"/>
     </row>
     <row r="25" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="51"/>
+      <c r="C25" s="57"/>
       <c r="D25" s="19">
         <v>14</v>
       </c>
@@ -1917,7 +1920,7 @@
       </c>
     </row>
     <row r="26" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="51"/>
+      <c r="C26" s="57"/>
       <c r="D26" s="19" t="s">
         <v>1</v>
       </c>
@@ -1972,7 +1975,7 @@
     </row>
     <row r="27" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27"/>
-      <c r="C27" s="51"/>
+      <c r="C27" s="57"/>
       <c r="D27" s="42" t="s">
         <v>94</v>
       </c>
@@ -1990,12 +1993,12 @@
       <c r="L27" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="53"/>
       <c r="O27" s="43"/>
-      <c r="P27" s="52"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="54"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="60"/>
       <c r="S27" s="42" t="s">
         <v>85</v>
       </c>
@@ -2208,45 +2211,45 @@
       </c>
       <c r="E31" s="43"/>
       <c r="F31" s="15"/>
-      <c r="G31" s="45" t="s">
+      <c r="G31" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="47"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="49"/>
       <c r="K31" s="16"/>
       <c r="L31" s="38" t="s">
         <v>18</v>
       </c>
       <c r="M31" s="16"/>
-      <c r="N31" s="45" t="s">
+      <c r="N31" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="O31" s="46"/>
-      <c r="P31" s="46"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="47"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="49"/>
       <c r="S31" s="40"/>
       <c r="T31" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="U31" s="44"/>
-      <c r="V31" s="44"/>
+      <c r="U31" s="53"/>
+      <c r="V31" s="53"/>
       <c r="W31" s="43"/>
-      <c r="X31" s="58"/>
-      <c r="Y31" s="59"/>
-      <c r="Z31" s="60"/>
+      <c r="X31" s="50"/>
+      <c r="Y31" s="51"/>
+      <c r="Z31" s="52"/>
       <c r="AA31" s="16"/>
-      <c r="AB31" s="55" t="s">
+      <c r="AB31" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="AC31" s="57"/>
+      <c r="AC31" s="46"/>
       <c r="AD31" s="18"/>
-      <c r="AE31" s="55" t="s">
+      <c r="AE31" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="AF31" s="56"/>
-      <c r="AG31" s="57"/>
+      <c r="AF31" s="45"/>
+      <c r="AG31" s="46"/>
       <c r="AH31" s="16"/>
     </row>
     <row r="32" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2428,12 +2431,12 @@
         <v>19</v>
       </c>
       <c r="J35" s="16"/>
-      <c r="K35" s="55" t="s">
+      <c r="K35" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="57"/>
+      <c r="L35" s="45"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="46"/>
       <c r="O35" s="15"/>
       <c r="P35" s="38" t="s">
         <v>20</v>
@@ -3626,13 +3629,12 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="AB31:AC31"/>
-    <mergeCell ref="AE31:AG31"/>
-    <mergeCell ref="N31:R31"/>
-    <mergeCell ref="X31:Z31"/>
-    <mergeCell ref="T31:W31"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="S27:T27"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="G31:J31"/>
@@ -3649,12 +3651,13 @@
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="P27:R27"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="AB31:AC31"/>
+    <mergeCell ref="AE31:AG31"/>
+    <mergeCell ref="N31:R31"/>
+    <mergeCell ref="X31:Z31"/>
+    <mergeCell ref="T31:W31"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -6056,7 +6059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B12089-A125-43C4-B991-1713BAF1DE71}">
   <dimension ref="B2:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -6220,8 +6223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE48A7C-8AF9-4A0B-A8FC-E8EB53F5818B}">
   <dimension ref="B2:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6330,7 +6333,7 @@
         <v>38</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E8" s="36" t="s">
         <v>44</v>
@@ -6356,7 +6359,7 @@
         <v>38</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="E9" s="36" t="s">
         <v>47</v>
@@ -6408,7 +6411,7 @@
         <v>38</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="E11" s="36" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
estados finalizado + diagrama classes (duvida com stor)
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TrabalhosPraticos\Projeto Aplicado\ipca_gym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB09AFA-CE89-4A06-B8A5-FEB13736269D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE7A5DE-F7C3-4236-9F41-222772DB47EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma_Projecto" sheetId="1" r:id="rId1"/>
@@ -358,7 +358,7 @@
     <t>To-Do</t>
   </si>
   <si>
-    <t>Doing</t>
+    <t>Doing(duvida com stor)</t>
   </si>
 </sst>
 </file>
@@ -780,13 +780,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -796,18 +790,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -829,6 +811,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1129,7 +1129,7 @@
   <dimension ref="A2:AP112"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1168,43 +1168,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="55"/>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="55"/>
-      <c r="AD2" s="55"/>
-      <c r="AE2" s="55"/>
-      <c r="AF2" s="55"/>
-      <c r="AG2" s="55"/>
-      <c r="AH2" s="55"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="49"/>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="49"/>
+      <c r="AH2" s="49"/>
     </row>
     <row r="5" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="50" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2">
@@ -1264,7 +1264,7 @@
       <c r="AH5"/>
     </row>
     <row r="6" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C6" s="56"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1322,7 +1322,7 @@
       <c r="AH6"/>
     </row>
     <row r="7" spans="2:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="56"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="42" t="s">
         <v>53</v>
       </c>
@@ -1341,7 +1341,7 @@
       <c r="K7" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="53"/>
+      <c r="L7" s="44"/>
       <c r="M7" s="43"/>
       <c r="N7" s="21" t="s">
         <v>57</v>
@@ -1402,7 +1402,7 @@
       <c r="AH8" s="12"/>
     </row>
     <row r="9" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="19">
@@ -1446,7 +1446,7 @@
       </c>
     </row>
     <row r="10" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C10" s="57"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="19" t="s">
         <v>5</v>
       </c>
@@ -1488,7 +1488,7 @@
       </c>
     </row>
     <row r="11" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="57"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="42" t="s">
         <v>24</v>
       </c>
@@ -1518,7 +1518,7 @@
       <c r="P11" s="15"/>
     </row>
     <row r="12" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C12" s="57"/>
+      <c r="C12" s="51"/>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
@@ -1535,7 +1535,7 @@
       <c r="AI12" s="7"/>
     </row>
     <row r="13" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C13" s="57"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="19">
         <v>14</v>
       </c>
@@ -1577,7 +1577,7 @@
       </c>
     </row>
     <row r="14" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C14" s="57"/>
+      <c r="C14" s="51"/>
       <c r="D14" s="27" t="s">
         <v>4</v>
       </c>
@@ -1624,13 +1624,13 @@
       <c r="AP14" s="1"/>
     </row>
     <row r="15" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="57"/>
+      <c r="C15" s="51"/>
       <c r="D15" s="20"/>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="47"/>
       <c r="H15" s="17"/>
       <c r="I15" s="42" t="s">
         <v>71</v>
@@ -1662,11 +1662,11 @@
     </row>
     <row r="16" spans="2:42" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="57"/>
+      <c r="C16" s="51"/>
     </row>
     <row r="17" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="57"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="19">
         <v>27</v>
       </c>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="18" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="57"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="19" t="s">
         <v>3</v>
       </c>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="19" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="57"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="42" t="s">
         <v>79</v>
       </c>
@@ -1719,7 +1719,7 @@
       <c r="B20" s="1"/>
     </row>
     <row r="21" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="57" t="s">
+      <c r="C21" s="51" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="19">
@@ -1764,7 +1764,7 @@
       <c r="AH21" s="12"/>
     </row>
     <row r="22" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="57"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="19" t="s">
         <v>6</v>
       </c>
@@ -1807,7 +1807,7 @@
       <c r="AH22" s="12"/>
     </row>
     <row r="23" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="57"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="21" t="s">
         <v>74</v>
       </c>
@@ -1832,7 +1832,7 @@
       <c r="AH23" s="12"/>
     </row>
     <row r="24" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="57"/>
+      <c r="C24" s="51"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
@@ -1866,7 +1866,7 @@
       <c r="AH24" s="14"/>
     </row>
     <row r="25" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="57"/>
+      <c r="C25" s="51"/>
       <c r="D25" s="19">
         <v>14</v>
       </c>
@@ -1920,7 +1920,7 @@
       </c>
     </row>
     <row r="26" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="57"/>
+      <c r="C26" s="51"/>
       <c r="D26" s="19" t="s">
         <v>1</v>
       </c>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="27" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27"/>
-      <c r="C27" s="57"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="42" t="s">
         <v>94</v>
       </c>
@@ -1993,12 +1993,12 @@
       <c r="L27" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="M27" s="53"/>
-      <c r="N27" s="53"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
       <c r="O27" s="43"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="59"/>
-      <c r="R27" s="60"/>
+      <c r="P27" s="52"/>
+      <c r="Q27" s="53"/>
+      <c r="R27" s="54"/>
       <c r="S27" s="42" t="s">
         <v>85</v>
       </c>
@@ -2211,45 +2211,45 @@
       </c>
       <c r="E31" s="43"/>
       <c r="F31" s="15"/>
-      <c r="G31" s="47" t="s">
+      <c r="G31" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="49"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="47"/>
       <c r="K31" s="16"/>
       <c r="L31" s="38" t="s">
         <v>18</v>
       </c>
       <c r="M31" s="16"/>
-      <c r="N31" s="47" t="s">
+      <c r="N31" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="O31" s="48"/>
-      <c r="P31" s="48"/>
-      <c r="Q31" s="48"/>
-      <c r="R31" s="49"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46"/>
+      <c r="R31" s="47"/>
       <c r="S31" s="40"/>
       <c r="T31" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="U31" s="53"/>
-      <c r="V31" s="53"/>
+      <c r="U31" s="44"/>
+      <c r="V31" s="44"/>
       <c r="W31" s="43"/>
-      <c r="X31" s="50"/>
-      <c r="Y31" s="51"/>
-      <c r="Z31" s="52"/>
+      <c r="X31" s="58"/>
+      <c r="Y31" s="59"/>
+      <c r="Z31" s="60"/>
       <c r="AA31" s="16"/>
-      <c r="AB31" s="44" t="s">
+      <c r="AB31" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="AC31" s="46"/>
+      <c r="AC31" s="57"/>
       <c r="AD31" s="18"/>
-      <c r="AE31" s="44" t="s">
+      <c r="AE31" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="AF31" s="45"/>
-      <c r="AG31" s="46"/>
+      <c r="AF31" s="56"/>
+      <c r="AG31" s="57"/>
       <c r="AH31" s="16"/>
     </row>
     <row r="32" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2431,12 +2431,12 @@
         <v>19</v>
       </c>
       <c r="J35" s="16"/>
-      <c r="K35" s="44" t="s">
+      <c r="K35" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="L35" s="45"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="46"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="57"/>
       <c r="O35" s="15"/>
       <c r="P35" s="38" t="s">
         <v>20</v>
@@ -3629,12 +3629,13 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="AB31:AC31"/>
+    <mergeCell ref="AE31:AG31"/>
+    <mergeCell ref="N31:R31"/>
+    <mergeCell ref="X31:Z31"/>
+    <mergeCell ref="T31:W31"/>
     <mergeCell ref="S27:T27"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="G31:J31"/>
@@ -3651,13 +3652,12 @@
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="P27:R27"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="AB31:AC31"/>
-    <mergeCell ref="AE31:AG31"/>
-    <mergeCell ref="N31:R31"/>
-    <mergeCell ref="X31:Z31"/>
-    <mergeCell ref="T31:W31"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -6060,7 +6060,7 @@
   <dimension ref="B2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6224,13 +6224,14 @@
   <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
@@ -6385,7 +6386,7 @@
         <v>38</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E10" s="36" t="s">
         <v>49</v>
@@ -6463,7 +6464,7 @@
         <v>38</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>100</v>
+        <v>39</v>
       </c>
       <c r="E13" s="36" t="s">
         <v>79</v>
@@ -6491,7 +6492,7 @@
   <dimension ref="B2:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update files (nada de novo)
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TrabalhosPraticos\Projeto Aplicado\ipca_gym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE7A5DE-F7C3-4236-9F41-222772DB47EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248AFDEC-B938-4D43-BC6F-CC684173C2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma_Projecto" sheetId="1" r:id="rId1"/>
@@ -358,7 +358,7 @@
     <t>To-Do</t>
   </si>
   <si>
-    <t>Doing(duvida com stor)</t>
+    <t>Done (duvida com stor)</t>
   </si>
 </sst>
 </file>
@@ -780,7 +780,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,6 +796,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -811,24 +829,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1168,43 +1168,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
-      <c r="AE2" s="49"/>
-      <c r="AF2" s="49"/>
-      <c r="AG2" s="49"/>
-      <c r="AH2" s="49"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="55"/>
+      <c r="AC2" s="55"/>
+      <c r="AD2" s="55"/>
+      <c r="AE2" s="55"/>
+      <c r="AF2" s="55"/>
+      <c r="AG2" s="55"/>
+      <c r="AH2" s="55"/>
     </row>
     <row r="5" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="56" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2">
@@ -1264,7 +1264,7 @@
       <c r="AH5"/>
     </row>
     <row r="6" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C6" s="50"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1322,7 +1322,7 @@
       <c r="AH6"/>
     </row>
     <row r="7" spans="2:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="50"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="42" t="s">
         <v>53</v>
       </c>
@@ -1341,7 +1341,7 @@
       <c r="K7" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="44"/>
+      <c r="L7" s="53"/>
       <c r="M7" s="43"/>
       <c r="N7" s="21" t="s">
         <v>57</v>
@@ -1402,7 +1402,7 @@
       <c r="AH8" s="12"/>
     </row>
     <row r="9" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="57" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="19">
@@ -1446,7 +1446,7 @@
       </c>
     </row>
     <row r="10" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C10" s="51"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="19" t="s">
         <v>5</v>
       </c>
@@ -1488,7 +1488,7 @@
       </c>
     </row>
     <row r="11" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="51"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="42" t="s">
         <v>24</v>
       </c>
@@ -1518,7 +1518,7 @@
       <c r="P11" s="15"/>
     </row>
     <row r="12" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C12" s="51"/>
+      <c r="C12" s="57"/>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
@@ -1535,7 +1535,7 @@
       <c r="AI12" s="7"/>
     </row>
     <row r="13" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C13" s="51"/>
+      <c r="C13" s="57"/>
       <c r="D13" s="19">
         <v>14</v>
       </c>
@@ -1577,7 +1577,7 @@
       </c>
     </row>
     <row r="14" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C14" s="51"/>
+      <c r="C14" s="57"/>
       <c r="D14" s="27" t="s">
         <v>4</v>
       </c>
@@ -1624,13 +1624,13 @@
       <c r="AP14" s="1"/>
     </row>
     <row r="15" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="51"/>
+      <c r="C15" s="57"/>
       <c r="D15" s="20"/>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="47"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="49"/>
       <c r="H15" s="17"/>
       <c r="I15" s="42" t="s">
         <v>71</v>
@@ -1662,11 +1662,11 @@
     </row>
     <row r="16" spans="2:42" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="51"/>
+      <c r="C16" s="57"/>
     </row>
     <row r="17" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="51"/>
+      <c r="C17" s="57"/>
       <c r="D17" s="19">
         <v>27</v>
       </c>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="18" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="51"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="19" t="s">
         <v>3</v>
       </c>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="19" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="51"/>
+      <c r="C19" s="57"/>
       <c r="D19" s="42" t="s">
         <v>79</v>
       </c>
@@ -1719,7 +1719,7 @@
       <c r="B20" s="1"/>
     </row>
     <row r="21" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="51" t="s">
+      <c r="C21" s="57" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="19">
@@ -1764,7 +1764,7 @@
       <c r="AH21" s="12"/>
     </row>
     <row r="22" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="51"/>
+      <c r="C22" s="57"/>
       <c r="D22" s="19" t="s">
         <v>6</v>
       </c>
@@ -1807,7 +1807,7 @@
       <c r="AH22" s="12"/>
     </row>
     <row r="23" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="51"/>
+      <c r="C23" s="57"/>
       <c r="D23" s="21" t="s">
         <v>74</v>
       </c>
@@ -1832,7 +1832,7 @@
       <c r="AH23" s="12"/>
     </row>
     <row r="24" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="51"/>
+      <c r="C24" s="57"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
@@ -1866,7 +1866,7 @@
       <c r="AH24" s="14"/>
     </row>
     <row r="25" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="51"/>
+      <c r="C25" s="57"/>
       <c r="D25" s="19">
         <v>14</v>
       </c>
@@ -1920,7 +1920,7 @@
       </c>
     </row>
     <row r="26" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="51"/>
+      <c r="C26" s="57"/>
       <c r="D26" s="19" t="s">
         <v>1</v>
       </c>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="27" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27"/>
-      <c r="C27" s="51"/>
+      <c r="C27" s="57"/>
       <c r="D27" s="42" t="s">
         <v>94</v>
       </c>
@@ -1993,12 +1993,12 @@
       <c r="L27" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="53"/>
       <c r="O27" s="43"/>
-      <c r="P27" s="52"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="54"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="60"/>
       <c r="S27" s="42" t="s">
         <v>85</v>
       </c>
@@ -2211,45 +2211,45 @@
       </c>
       <c r="E31" s="43"/>
       <c r="F31" s="15"/>
-      <c r="G31" s="45" t="s">
+      <c r="G31" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="47"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="49"/>
       <c r="K31" s="16"/>
       <c r="L31" s="38" t="s">
         <v>18</v>
       </c>
       <c r="M31" s="16"/>
-      <c r="N31" s="45" t="s">
+      <c r="N31" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="O31" s="46"/>
-      <c r="P31" s="46"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="47"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="49"/>
       <c r="S31" s="40"/>
       <c r="T31" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="U31" s="44"/>
-      <c r="V31" s="44"/>
+      <c r="U31" s="53"/>
+      <c r="V31" s="53"/>
       <c r="W31" s="43"/>
-      <c r="X31" s="58"/>
-      <c r="Y31" s="59"/>
-      <c r="Z31" s="60"/>
+      <c r="X31" s="50"/>
+      <c r="Y31" s="51"/>
+      <c r="Z31" s="52"/>
       <c r="AA31" s="16"/>
-      <c r="AB31" s="55" t="s">
+      <c r="AB31" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="AC31" s="57"/>
+      <c r="AC31" s="46"/>
       <c r="AD31" s="18"/>
-      <c r="AE31" s="55" t="s">
+      <c r="AE31" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="AF31" s="56"/>
-      <c r="AG31" s="57"/>
+      <c r="AF31" s="45"/>
+      <c r="AG31" s="46"/>
       <c r="AH31" s="16"/>
     </row>
     <row r="32" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2431,12 +2431,12 @@
         <v>19</v>
       </c>
       <c r="J35" s="16"/>
-      <c r="K35" s="55" t="s">
+      <c r="K35" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="57"/>
+      <c r="L35" s="45"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="46"/>
       <c r="O35" s="15"/>
       <c r="P35" s="38" t="s">
         <v>20</v>
@@ -3629,13 +3629,12 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="AB31:AC31"/>
-    <mergeCell ref="AE31:AG31"/>
-    <mergeCell ref="N31:R31"/>
-    <mergeCell ref="X31:Z31"/>
-    <mergeCell ref="T31:W31"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="S27:T27"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="G31:J31"/>
@@ -3652,12 +3651,13 @@
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="P27:R27"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="AB31:AC31"/>
+    <mergeCell ref="AE31:AG31"/>
+    <mergeCell ref="N31:R31"/>
+    <mergeCell ref="X31:Z31"/>
+    <mergeCell ref="T31:W31"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -6224,7 +6224,7 @@
   <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Organização de Pastas + update Especificação
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TrabalhosPraticos\Projeto Aplicado\ipca_gym\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TrabalhosPraticos\Projeto_Aplicado\ipca_gym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E934F8-916F-498B-A426-972BEE80C432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979B2C7D-56EA-4D60-9265-606B6B8A0EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma_Projecto" sheetId="1" r:id="rId1"/>
@@ -780,7 +780,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,6 +796,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -811,24 +829,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1128,83 +1128,83 @@
   </sheetPr>
   <dimension ref="A2:AP112"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="F4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="1.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="1.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="61" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="40.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="27.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="33.42578125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="19.140625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="12.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="40.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="49.5546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="23.88671875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="27.109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="33.44140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="19.109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="14.44140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="14.109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.88671875" style="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" customWidth="1"/>
     <col min="26" max="27" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="27.7109375" style="1" customWidth="1"/>
-    <col min="29" max="29" width="8.5703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="14.42578125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="16.42578125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="15.7109375" style="1" customWidth="1"/>
-    <col min="33" max="33" width="18.5703125" style="1" customWidth="1"/>
-    <col min="34" max="34" width="25.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="27.6640625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="8.5546875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="14.44140625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="16.44140625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="15.6640625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="18.5546875" style="1" customWidth="1"/>
+    <col min="34" max="34" width="25.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="48" t="s">
+    <row r="2" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
-      <c r="AE2" s="49"/>
-      <c r="AF2" s="49"/>
-      <c r="AG2" s="49"/>
-      <c r="AH2" s="49"/>
-    </row>
-    <row r="5" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C5" s="50" t="s">
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="55"/>
+      <c r="AC2" s="55"/>
+      <c r="AD2" s="55"/>
+      <c r="AE2" s="55"/>
+      <c r="AF2" s="55"/>
+      <c r="AG2" s="55"/>
+      <c r="AH2" s="55"/>
+    </row>
+    <row r="5" spans="2:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C5" s="56" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2">
@@ -1263,8 +1263,8 @@
       <c r="AG5"/>
       <c r="AH5"/>
     </row>
-    <row r="6" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C6" s="50"/>
+    <row r="6" spans="2:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C6" s="56"/>
       <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1321,8 +1321,8 @@
       <c r="AG6"/>
       <c r="AH6"/>
     </row>
-    <row r="7" spans="2:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="50"/>
+    <row r="7" spans="2:42" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="56"/>
       <c r="D7" s="42" t="s">
         <v>53</v>
       </c>
@@ -1341,7 +1341,7 @@
       <c r="K7" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="44"/>
+      <c r="L7" s="53"/>
       <c r="M7" s="43"/>
       <c r="N7" s="21" t="s">
         <v>57</v>
@@ -1367,7 +1367,7 @@
       <c r="AG7"/>
       <c r="AH7"/>
     </row>
-    <row r="8" spans="2:42" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:42" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
@@ -1401,8 +1401,8 @@
       <c r="AG8" s="12"/>
       <c r="AH8" s="12"/>
     </row>
-    <row r="9" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C9" s="51" t="s">
+    <row r="9" spans="2:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C9" s="57" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="19">
@@ -1445,8 +1445,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C10" s="51"/>
+    <row r="10" spans="2:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C10" s="57"/>
       <c r="D10" s="19" t="s">
         <v>5</v>
       </c>
@@ -1487,8 +1487,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="51"/>
+    <row r="11" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="57"/>
       <c r="D11" s="42" t="s">
         <v>24</v>
       </c>
@@ -1517,8 +1517,8 @@
       </c>
       <c r="P11" s="15"/>
     </row>
-    <row r="12" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C12" s="51"/>
+    <row r="12" spans="2:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C12" s="57"/>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
@@ -1534,8 +1534,8 @@
       <c r="AH12" s="13"/>
       <c r="AI12" s="7"/>
     </row>
-    <row r="13" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C13" s="51"/>
+    <row r="13" spans="2:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C13" s="57"/>
       <c r="D13" s="19">
         <v>14</v>
       </c>
@@ -1576,8 +1576,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:42" ht="15" x14ac:dyDescent="0.25">
-      <c r="C14" s="51"/>
+    <row r="14" spans="2:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C14" s="57"/>
       <c r="D14" s="27" t="s">
         <v>4</v>
       </c>
@@ -1623,14 +1623,14 @@
       <c r="AO14" s="1"/>
       <c r="AP14" s="1"/>
     </row>
-    <row r="15" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="51"/>
+    <row r="15" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="57"/>
       <c r="D15" s="20"/>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="47"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="49"/>
       <c r="H15" s="17"/>
       <c r="I15" s="42" t="s">
         <v>71</v>
@@ -1660,13 +1660,13 @@
       <c r="AO15" s="1"/>
       <c r="AP15" s="1"/>
     </row>
-    <row r="16" spans="2:42" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:42" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
-      <c r="C16" s="51"/>
-    </row>
-    <row r="17" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="57"/>
+    </row>
+    <row r="17" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="51"/>
+      <c r="C17" s="57"/>
       <c r="D17" s="19">
         <v>27</v>
       </c>
@@ -1683,9 +1683,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="51"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="19" t="s">
         <v>3</v>
       </c>
@@ -1702,9 +1702,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="51"/>
+      <c r="C19" s="57"/>
       <c r="D19" s="42" t="s">
         <v>79</v>
       </c>
@@ -1715,11 +1715,11 @@
       <c r="G19" s="43"/>
       <c r="H19" s="15"/>
     </row>
-    <row r="20" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="51" t="s">
+    <row r="21" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="57" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="19">
@@ -1763,8 +1763,8 @@
       </c>
       <c r="AH21" s="12"/>
     </row>
-    <row r="22" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="51"/>
+    <row r="22" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="57"/>
       <c r="D22" s="19" t="s">
         <v>6</v>
       </c>
@@ -1806,8 +1806,8 @@
       </c>
       <c r="AH22" s="12"/>
     </row>
-    <row r="23" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="51"/>
+    <row r="23" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="57"/>
       <c r="D23" s="21" t="s">
         <v>74</v>
       </c>
@@ -1831,8 +1831,8 @@
       <c r="P23" s="16"/>
       <c r="AH23" s="12"/>
     </row>
-    <row r="24" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="51"/>
+    <row r="24" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="57"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
@@ -1865,8 +1865,8 @@
       <c r="AG24" s="14"/>
       <c r="AH24" s="14"/>
     </row>
-    <row r="25" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="51"/>
+    <row r="25" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="57"/>
       <c r="D25" s="19">
         <v>14</v>
       </c>
@@ -1919,8 +1919,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="51"/>
+    <row r="26" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="57"/>
       <c r="D26" s="19" t="s">
         <v>1</v>
       </c>
@@ -1973,9 +1973,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27"/>
-      <c r="C27" s="51"/>
+      <c r="C27" s="57"/>
       <c r="D27" s="42" t="s">
         <v>94</v>
       </c>
@@ -1993,21 +1993,21 @@
       <c r="L27" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="53"/>
       <c r="O27" s="43"/>
-      <c r="P27" s="52"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="54"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="60"/>
       <c r="S27" s="42" t="s">
         <v>85</v>
       </c>
       <c r="T27" s="43"/>
     </row>
-    <row r="28" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28"/>
     </row>
-    <row r="29" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29"/>
       <c r="C29" s="10" t="s">
         <v>9</v>
@@ -2106,7 +2106,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30"/>
       <c r="C30" s="11"/>
       <c r="D30" s="2" t="s">
@@ -2203,7 +2203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:34" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:34" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31"/>
       <c r="C31" s="12"/>
       <c r="D31" s="42" t="s">
@@ -2211,48 +2211,48 @@
       </c>
       <c r="E31" s="43"/>
       <c r="F31" s="15"/>
-      <c r="G31" s="45" t="s">
+      <c r="G31" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="47"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="49"/>
       <c r="K31" s="16"/>
       <c r="L31" s="38" t="s">
         <v>18</v>
       </c>
       <c r="M31" s="16"/>
-      <c r="N31" s="45" t="s">
+      <c r="N31" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="O31" s="46"/>
-      <c r="P31" s="46"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="47"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="49"/>
       <c r="S31" s="40"/>
       <c r="T31" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="U31" s="44"/>
-      <c r="V31" s="44"/>
+      <c r="U31" s="53"/>
+      <c r="V31" s="53"/>
       <c r="W31" s="43"/>
-      <c r="X31" s="58"/>
-      <c r="Y31" s="59"/>
-      <c r="Z31" s="60"/>
+      <c r="X31" s="50"/>
+      <c r="Y31" s="51"/>
+      <c r="Z31" s="52"/>
       <c r="AA31" s="16"/>
-      <c r="AB31" s="55" t="s">
+      <c r="AB31" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="AC31" s="57"/>
+      <c r="AC31" s="46"/>
       <c r="AD31" s="18"/>
-      <c r="AE31" s="55" t="s">
+      <c r="AE31" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="AF31" s="56"/>
-      <c r="AG31" s="57"/>
+      <c r="AF31" s="45"/>
+      <c r="AG31" s="46"/>
       <c r="AH31" s="16"/>
     </row>
-    <row r="32" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -2287,7 +2287,7 @@
       <c r="AG32" s="12"/>
       <c r="AH32" s="12"/>
     </row>
-    <row r="33" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33"/>
       <c r="C33" s="10" t="s">
         <v>10</v>
@@ -2353,7 +2353,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34"/>
       <c r="C34" s="11"/>
       <c r="D34" s="2" t="s">
@@ -2417,7 +2417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35"/>
       <c r="C35" s="12"/>
       <c r="D35" s="16"/>
@@ -2431,12 +2431,12 @@
         <v>19</v>
       </c>
       <c r="J35" s="16"/>
-      <c r="K35" s="55" t="s">
+      <c r="K35" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="57"/>
+      <c r="L35" s="45"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="46"/>
       <c r="O35" s="15"/>
       <c r="P35" s="38" t="s">
         <v>20</v>
@@ -2453,7 +2453,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
@@ -2461,7 +2461,7 @@
       <c r="F36"/>
       <c r="G36"/>
     </row>
-    <row r="37" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
@@ -2469,7 +2469,7 @@
       <c r="F37"/>
       <c r="G37"/>
     </row>
-    <row r="38" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
@@ -2477,7 +2477,7 @@
       <c r="F38"/>
       <c r="G38"/>
     </row>
-    <row r="39" spans="1:39" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39" t="s">
@@ -2490,7 +2490,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
@@ -2498,7 +2498,7 @@
       <c r="F40"/>
       <c r="G40"/>
     </row>
-    <row r="41" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
@@ -2506,7 +2506,7 @@
       <c r="F41"/>
       <c r="G41"/>
     </row>
-    <row r="42" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42"/>
@@ -2514,7 +2514,7 @@
       <c r="F42"/>
       <c r="G42"/>
     </row>
-    <row r="43" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -2549,7 +2549,7 @@
       <c r="AG43" s="4"/>
       <c r="AH43"/>
     </row>
-    <row r="44" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44" s="6"/>
@@ -2589,7 +2589,7 @@
       <c r="AL44"/>
       <c r="AM44"/>
     </row>
-    <row r="45" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45"/>
       <c r="AI45" s="4"/>
       <c r="AJ45" s="4"/>
@@ -2597,7 +2597,7 @@
       <c r="AL45" s="4"/>
       <c r="AM45" s="4"/>
     </row>
-    <row r="46" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -2608,91 +2608,91 @@
       <c r="AL46" s="4"/>
       <c r="AM46" s="4"/>
     </row>
-    <row r="47" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
     </row>
-    <row r="48" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:39" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
     </row>
-    <row r="49" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
     </row>
-    <row r="51" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
     </row>
-    <row r="52" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
     </row>
-    <row r="53" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
     </row>
-    <row r="54" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
     </row>
-    <row r="55" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
     </row>
-    <row r="56" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
     </row>
-    <row r="57" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
     </row>
-    <row r="58" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
     </row>
-    <row r="59" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59"/>
       <c r="C59"/>
@@ -2728,7 +2728,7 @@
       <c r="AG59" s="1"/>
       <c r="AH59" s="1"/>
     </row>
-    <row r="60" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
@@ -2769,14 +2769,14 @@
       <c r="AL60" s="4"/>
       <c r="AM60" s="4"/>
     </row>
-    <row r="61" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AI61" s="4"/>
       <c r="AJ61" s="4"/>
       <c r="AK61" s="4"/>
       <c r="AL61" s="4"/>
       <c r="AM61" s="4"/>
     </row>
-    <row r="62" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62"/>
       <c r="AI62" s="4"/>
       <c r="AJ62" s="4"/>
@@ -2784,7 +2784,7 @@
       <c r="AL62" s="4"/>
       <c r="AM62" s="4"/>
     </row>
-    <row r="63" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63"/>
       <c r="AI63" s="4"/>
       <c r="AJ63" s="4"/>
@@ -2792,7 +2792,7 @@
       <c r="AL63" s="4"/>
       <c r="AM63" s="4"/>
     </row>
-    <row r="64" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64"/>
       <c r="AI64"/>
       <c r="AJ64"/>
@@ -2801,7 +2801,7 @@
       <c r="AM64"/>
       <c r="AN64"/>
     </row>
-    <row r="65" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65"/>
       <c r="AI65"/>
       <c r="AJ65"/>
@@ -2810,7 +2810,7 @@
       <c r="AM65"/>
       <c r="AN65"/>
     </row>
-    <row r="66" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66"/>
       <c r="AI66"/>
       <c r="AJ66"/>
@@ -2819,7 +2819,7 @@
       <c r="AM66"/>
       <c r="AN66"/>
     </row>
-    <row r="67" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67"/>
       <c r="AI67"/>
       <c r="AJ67"/>
@@ -2828,7 +2828,7 @@
       <c r="AM67"/>
       <c r="AN67"/>
     </row>
-    <row r="68" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68"/>
       <c r="AI68"/>
       <c r="AJ68"/>
@@ -2837,7 +2837,7 @@
       <c r="AM68"/>
       <c r="AN68"/>
     </row>
-    <row r="69" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69"/>
       <c r="AI69"/>
       <c r="AJ69"/>
@@ -2846,7 +2846,7 @@
       <c r="AM69"/>
       <c r="AN69"/>
     </row>
-    <row r="70" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70"/>
       <c r="AI70"/>
       <c r="AJ70"/>
@@ -2855,7 +2855,7 @@
       <c r="AM70"/>
       <c r="AN70"/>
     </row>
-    <row r="71" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
@@ -2867,43 +2867,43 @@
       <c r="AM71"/>
       <c r="AN71"/>
     </row>
-    <row r="72" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
       <c r="D72"/>
     </row>
-    <row r="73" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
     </row>
-    <row r="74" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
     </row>
-    <row r="75" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
     </row>
-    <row r="76" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76"/>
     </row>
-    <row r="77" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77"/>
     </row>
-    <row r="78" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78"/>
     </row>
-    <row r="79" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79"/>
     </row>
-    <row r="80" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:40" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80" s="4"/>
@@ -2912,7 +2912,7 @@
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
     </row>
-    <row r="81" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81" s="4"/>
@@ -2921,7 +2921,7 @@
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
     </row>
-    <row r="82" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82" s="4"/>
@@ -2930,7 +2930,7 @@
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
     </row>
-    <row r="83" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83" s="4"/>
@@ -2939,7 +2939,7 @@
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
     </row>
-    <row r="84" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84" s="4"/>
@@ -2948,7 +2948,7 @@
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
     </row>
-    <row r="85" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85" s="4"/>
@@ -2957,7 +2957,7 @@
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
     </row>
-    <row r="86" spans="1:34" s="3" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:34" s="3" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86" s="4"/>
@@ -2966,7 +2966,7 @@
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
     </row>
-    <row r="87" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87" s="4"/>
@@ -2975,7 +2975,7 @@
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
     </row>
-    <row r="88" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88" s="4"/>
@@ -2984,7 +2984,7 @@
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
     </row>
-    <row r="89" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89" s="4"/>
@@ -2993,7 +2993,7 @@
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
     </row>
-    <row r="90" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90" s="4"/>
@@ -3002,7 +3002,7 @@
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
     </row>
-    <row r="91" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
@@ -3038,7 +3038,7 @@
       <c r="AG91"/>
       <c r="AH91"/>
     </row>
-    <row r="92" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
@@ -3073,7 +3073,7 @@
       <c r="AG92" s="3"/>
       <c r="AH92" s="3"/>
     </row>
-    <row r="93" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:34" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4"/>
       <c r="B93" s="1"/>
       <c r="C93"/>
@@ -3109,7 +3109,7 @@
       <c r="AG93"/>
       <c r="AH93"/>
     </row>
-    <row r="94" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -3145,7 +3145,7 @@
       <c r="AG94"/>
       <c r="AH94"/>
     </row>
-    <row r="95" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -3181,7 +3181,7 @@
       <c r="AG95"/>
       <c r="AH95"/>
     </row>
-    <row r="96" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="D96"/>
       <c r="F96"/>
@@ -3211,7 +3211,7 @@
       <c r="AG96"/>
       <c r="AH96"/>
     </row>
-    <row r="97" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D97"/>
       <c r="F97"/>
       <c r="G97"/>
@@ -3240,7 +3240,7 @@
       <c r="AG97"/>
       <c r="AH97"/>
     </row>
-    <row r="98" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D98"/>
       <c r="F98"/>
       <c r="G98"/>
@@ -3269,7 +3269,7 @@
       <c r="AG98"/>
       <c r="AH98"/>
     </row>
-    <row r="99" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D99"/>
       <c r="F99"/>
       <c r="G99"/>
@@ -3298,7 +3298,7 @@
       <c r="AG99"/>
       <c r="AH99"/>
     </row>
-    <row r="100" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D100"/>
       <c r="F100"/>
       <c r="G100"/>
@@ -3327,7 +3327,7 @@
       <c r="AG100"/>
       <c r="AH100"/>
     </row>
-    <row r="101" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D101"/>
       <c r="F101"/>
       <c r="G101"/>
@@ -3357,7 +3357,7 @@
       <c r="AG101"/>
       <c r="AH101"/>
     </row>
-    <row r="102" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D102"/>
       <c r="F102"/>
       <c r="G102"/>
@@ -3387,7 +3387,7 @@
       <c r="AG102"/>
       <c r="AH102"/>
     </row>
-    <row r="103" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D103"/>
       <c r="F103"/>
       <c r="G103"/>
@@ -3417,7 +3417,7 @@
       <c r="AG103"/>
       <c r="AH103"/>
     </row>
-    <row r="104" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D104"/>
       <c r="F104"/>
       <c r="G104"/>
@@ -3447,7 +3447,7 @@
       <c r="AG104"/>
       <c r="AH104"/>
     </row>
-    <row r="105" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D105"/>
       <c r="F105"/>
       <c r="G105"/>
@@ -3477,7 +3477,7 @@
       <c r="AG105"/>
       <c r="AH105"/>
     </row>
-    <row r="106" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D106"/>
       <c r="F106"/>
       <c r="G106"/>
@@ -3507,7 +3507,7 @@
       <c r="AG106"/>
       <c r="AH106"/>
     </row>
-    <row r="107" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D107"/>
       <c r="F107"/>
       <c r="G107"/>
@@ -3537,7 +3537,7 @@
       <c r="AG107"/>
       <c r="AH107"/>
     </row>
-    <row r="108" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="R108"/>
@@ -3558,7 +3558,7 @@
       <c r="AG108"/>
       <c r="AH108"/>
     </row>
-    <row r="109" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3580,7 +3580,7 @@
       <c r="AG109"/>
       <c r="AH109"/>
     </row>
-    <row r="110" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3602,7 +3602,7 @@
       <c r="AG110"/>
       <c r="AH110"/>
     </row>
-    <row r="111" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3624,18 +3624,17 @@
       <c r="AG111"/>
       <c r="AH111"/>
     </row>
-    <row r="112" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="AB31:AC31"/>
-    <mergeCell ref="AE31:AG31"/>
-    <mergeCell ref="N31:R31"/>
-    <mergeCell ref="X31:Z31"/>
-    <mergeCell ref="T31:W31"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="S27:T27"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="G31:J31"/>
@@ -3652,12 +3651,13 @@
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="P27:R27"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="AB31:AC31"/>
+    <mergeCell ref="AE31:AG31"/>
+    <mergeCell ref="N31:R31"/>
+    <mergeCell ref="X31:Z31"/>
+    <mergeCell ref="T31:W31"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -3685,16 +3685,16 @@
       <selection activeCell="D8" sqref="D8:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -3708,7 +3708,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -3718,7 +3718,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -3732,7 +3732,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -3746,7 +3746,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -3756,7 +3756,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -3866,16 +3866,16 @@
       <selection activeCell="D8" sqref="D8:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -3889,7 +3889,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -3899,7 +3899,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -3913,7 +3913,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -3927,7 +3927,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -3937,7 +3937,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -4038,17 +4038,17 @@
       <selection activeCell="D8" sqref="D8:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -4062,7 +4062,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -4072,7 +4072,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -4086,7 +4086,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -4100,7 +4100,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -4110,7 +4110,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -4219,16 +4219,16 @@
       <selection activeCell="D8" sqref="D8:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -4242,7 +4242,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -4252,7 +4252,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -4266,7 +4266,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -4280,7 +4280,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -4290,7 +4290,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>88</v>
       </c>
@@ -4396,17 +4396,17 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -4420,7 +4420,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -4430,7 +4430,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -4444,7 +4444,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -4458,7 +4458,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -4468,7 +4468,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -4569,17 +4569,17 @@
       <selection activeCell="D9" sqref="D9:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28"/>
       <c r="C2" s="29"/>
       <c r="D2" s="30"/>
@@ -4589,7 +4589,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="28" t="s">
         <v>26</v>
       </c>
@@ -4603,7 +4603,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="31"/>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -4613,7 +4613,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>28</v>
       </c>
@@ -4627,7 +4627,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="28" t="s">
         <v>29</v>
       </c>
@@ -4641,7 +4641,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
@@ -4651,7 +4651,7 @@
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="33" t="s">
         <v>30</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>1</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>2</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="34">
         <v>3</v>
       </c>
@@ -4752,16 +4752,16 @@
       <selection activeCell="D8" sqref="D8:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -4775,7 +4775,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -4785,7 +4785,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -4799,7 +4799,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -4813,7 +4813,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -4823,7 +4823,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -4932,16 +4932,16 @@
       <selection activeCell="D8" sqref="D8:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -4955,7 +4955,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -4965,7 +4965,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -4979,7 +4979,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -4993,7 +4993,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -5003,7 +5003,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -5104,16 +5104,16 @@
       <selection activeCell="D8" sqref="D8:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -5127,7 +5127,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -5137,7 +5137,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -5151,7 +5151,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -5165,7 +5165,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -5175,7 +5175,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -5227,7 +5227,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -5263,7 +5263,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F14" s="41"/>
     </row>
   </sheetData>
@@ -5279,17 +5279,17 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -5303,7 +5303,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -5313,7 +5313,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -5327,7 +5327,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -5341,7 +5341,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -5351,7 +5351,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -5403,7 +5403,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -5468,17 +5468,17 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -5492,7 +5492,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -5502,7 +5502,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -5516,7 +5516,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -5530,7 +5530,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -5540,7 +5540,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -5566,7 +5566,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -5657,17 +5657,17 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -5681,7 +5681,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -5691,7 +5691,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -5705,7 +5705,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -5719,7 +5719,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -5729,7 +5729,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -5781,7 +5781,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -5846,19 +5846,19 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -5872,7 +5872,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -5882,7 +5882,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -5896,7 +5896,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -5910,7 +5910,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -5920,7 +5920,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="34">
         <v>4</v>
       </c>
@@ -6063,18 +6063,18 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -6088,7 +6088,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -6098,7 +6098,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -6112,7 +6112,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -6126,7 +6126,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -6136,7 +6136,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -6227,18 +6227,18 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -6252,7 +6252,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -6262,7 +6262,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -6276,7 +6276,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -6290,7 +6290,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -6300,7 +6300,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -6326,7 +6326,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -6378,7 +6378,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="34">
         <v>4</v>
       </c>
@@ -6430,7 +6430,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="34">
         <v>5</v>
       </c>
@@ -6456,7 +6456,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="34">
         <v>6</v>
       </c>
@@ -6495,18 +6495,18 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -6520,7 +6520,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -6530,7 +6530,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -6544,7 +6544,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -6558,7 +6558,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -6568,7 +6568,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -6620,7 +6620,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>
@@ -6685,16 +6685,16 @@
       <selection activeCell="D8" sqref="D8:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>26</v>
       </c>
@@ -6708,7 +6708,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="31"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -6718,7 +6718,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
@@ -6732,7 +6732,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
@@ -6746,7 +6746,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -6756,7 +6756,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>30</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="34">
         <v>1</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="34">
         <v>2</v>
       </c>
@@ -6834,7 +6834,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="34">
         <v>3</v>
       </c>

</xml_diff>